<commit_message>
neueste Versionen, Dokumentation und Arduino Code
</commit_message>
<xml_diff>
--- a/Dokumentation/Dokumentation_Projekt-Steuerung_Autonom-Fahrendes-Auto_cargroup03_After_9f32617dcf09bb7ac3d91f3f63ed8d08ef1232e2(1).xlsx
+++ b/Dokumentation/Dokumentation_Projekt-Steuerung_Autonom-Fahrendes-Auto_cargroup03_After_9f32617dcf09bb7ac3d91f3f63ed8d08ef1232e2(1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\001146\Documents\group-03\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\190031\Documents\group-03\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8865509-D6C5-4188-B237-90DCE167731C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7B938E-5201-4D11-8474-14E449B7D306}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="247">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1173,6 +1173,12 @@
   </si>
   <si>
     <t>Code fürs fahren durch die Teststrecke programmiert, funktioniert noch nicht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neuen Code für das Fahren durch die Strecke programmiert, hat noch Probleme </t>
+  </si>
+  <si>
+    <t>Motoren hatten Probleme, Verkabelung war falsch, wurde verbessert</t>
   </si>
 </sst>
 </file>
@@ -1565,7 +1571,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1916,12 +1922,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1930,36 +1969,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2470,14 +2479,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="132" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2526,10 +2535,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="121" t="s">
+      <c r="E7" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="121"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2540,8 +2549,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2552,8 +2561,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2564,8 +2573,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="135"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2576,8 +2585,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="129"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2598,49 +2607,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="126"/>
-      <c r="C15" s="126"/>
-      <c r="D15" s="126"/>
-      <c r="E15" s="126"/>
-      <c r="F15" s="126"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="127"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="127"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="127"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="127"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="127"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="127"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="127"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="131"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="131"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="132"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="132"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2653,64 +2662,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="133" t="s">
+      <c r="A23" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="133"/>
-      <c r="C23" s="133"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="133"/>
-      <c r="F23" s="133"/>
+      <c r="B23" s="126"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="121" t="s">
+      <c r="A26" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="121"/>
-      <c r="C26" s="121"/>
-      <c r="D26" s="121" t="s">
+      <c r="B26" s="127"/>
+      <c r="C26" s="127"/>
+      <c r="D26" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="121"/>
-      <c r="F26" s="121"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="129" t="s">
+      <c r="A27" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="129"/>
-      <c r="C27" s="129"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="128" t="s">
+      <c r="A28" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="128"/>
-      <c r="C28" s="128"/>
-      <c r="D28" s="129" t="s">
+      <c r="B28" s="121"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="122" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="129"/>
-      <c r="F28" s="129"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="122"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="130" t="s">
+      <c r="A29" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="130"/>
-      <c r="C29" s="130"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="131"/>
-      <c r="F29" s="131"/>
+      <c r="B29" s="123"/>
+      <c r="C29" s="123"/>
+      <c r="D29" s="124"/>
+      <c r="E29" s="124"/>
+      <c r="F29" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2721,16 +2740,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2745,8 +2754,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,11 +2767,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="137" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
     </row>
     <row r="3" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -3009,15 +3018,27 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="105"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="105"/>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>45334</v>
+      </c>
+      <c r="B25" s="41">
+        <v>2</v>
+      </c>
+      <c r="C25" s="105" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>45334</v>
+      </c>
+      <c r="B26" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="105" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
@@ -3070,8 +3091,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,11 +3104,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="137" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3353,15 +3374,27 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="2"/>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="40">
+        <v>45334</v>
+      </c>
+      <c r="B27" s="41">
+        <v>2</v>
+      </c>
+      <c r="C27" s="120" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="40">
+        <v>45334</v>
+      </c>
+      <c r="B28" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="120" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
@@ -3475,29 +3508,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="136" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="135"/>
+      <c r="C3" s="136"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="135"/>
+      <c r="C4" s="136"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="135"/>
+      <c r="C5" s="136"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3708,7 +3741,7 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3720,11 +3753,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -3732,18 +3765,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
+      <c r="B3" s="138"/>
+      <c r="C3" s="138"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="139" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="138"/>
-      <c r="C4" s="138"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="139"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -4019,14 +4052,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4319,16 +4352,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="132" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5008,19 +5041,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -5684,16 +5717,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="137" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -6469,71 +6502,71 @@
       <c r="A21" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="142" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="142"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="101" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="C22" s="142"/>
-      <c r="D22" s="142"/>
+      <c r="C22" s="143"/>
+      <c r="D22" s="143"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>189</v>
       </c>
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="143" t="s">
         <v>190</v>
       </c>
-      <c r="C23" s="142"/>
-      <c r="D23" s="142"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="143"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="101" t="s">
         <v>191</v>
       </c>
-      <c r="B24" s="142" t="s">
+      <c r="B24" s="143" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="142"/>
-      <c r="D24" s="142"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="143"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
-      <c r="B25" s="140"/>
-      <c r="C25" s="140"/>
-      <c r="D25" s="140"/>
+      <c r="B25" s="141"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="141"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="98"/>
-      <c r="B26" s="140"/>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
+      <c r="B26" s="141"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="98"/>
-      <c r="B27" s="140"/>
-      <c r="C27" s="140"/>
-      <c r="D27" s="140"/>
+      <c r="B27" s="141"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
-      <c r="B28" s="140"/>
-      <c r="C28" s="140"/>
-      <c r="D28" s="140"/>
+      <c r="B28" s="141"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="98"/>
-      <c r="B29" s="140"/>
-      <c r="C29" s="140"/>
-      <c r="D29" s="140"/>
+      <c r="B29" s="141"/>
+      <c r="C29" s="141"/>
+      <c r="D29" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
neuester stand vom 260224
</commit_message>
<xml_diff>
--- a/Dokumentation/Dokumentation_Projekt-Steuerung_Autonom-Fahrendes-Auto_cargroup03_After_9f32617dcf09bb7ac3d91f3f63ed8d08ef1232e2(1).xlsx
+++ b/Dokumentation/Dokumentation_Projekt-Steuerung_Autonom-Fahrendes-Auto_cargroup03_After_9f32617dcf09bb7ac3d91f3f63ed8d08ef1232e2(1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\190031\Documents\group-03\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7B938E-5201-4D11-8474-14E449B7D306}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B57309-95B0-4FDE-86A4-AAD04D922923}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="249">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1179,6 +1179,12 @@
   </si>
   <si>
     <t>Motoren hatten Probleme, Verkabelung war falsch, wurde verbessert</t>
+  </si>
+  <si>
+    <t>Konzept überlegt und Flussdiagramm gezeicnet</t>
+  </si>
+  <si>
+    <t>Konzept als Code umgesetzt noch fehlerhaft</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1577,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1925,6 +1931,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1943,32 +1976,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2479,14 +2488,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="122" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2535,10 +2544,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="127" t="s">
+      <c r="E7" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="127"/>
+      <c r="F7" s="123"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2549,8 +2558,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
+      <c r="E8" s="124"/>
+      <c r="F8" s="124"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2561,8 +2570,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="125"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2573,8 +2582,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2585,8 +2594,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129"/>
+      <c r="E11" s="127"/>
+      <c r="F11" s="127"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2607,49 +2616,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="130"/>
-      <c r="C15" s="130"/>
-      <c r="D15" s="130"/>
-      <c r="E15" s="130"/>
-      <c r="F15" s="130"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
+      <c r="B16" s="129"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="129"/>
+      <c r="E16" s="129"/>
+      <c r="F16" s="129"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="129"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="131"/>
-      <c r="C18" s="131"/>
-      <c r="D18" s="131"/>
-      <c r="E18" s="131"/>
-      <c r="F18" s="131"/>
+      <c r="B18" s="129"/>
+      <c r="C18" s="129"/>
+      <c r="D18" s="129"/>
+      <c r="E18" s="129"/>
+      <c r="F18" s="129"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="125"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="134"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="134"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2662,74 +2671,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="126" t="s">
+      <c r="A23" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="126"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="126"/>
-      <c r="F23" s="126"/>
+      <c r="B23" s="135"/>
+      <c r="C23" s="135"/>
+      <c r="D23" s="135"/>
+      <c r="E23" s="135"/>
+      <c r="F23" s="135"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="127" t="s">
+      <c r="A26" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="127"/>
-      <c r="C26" s="127"/>
-      <c r="D26" s="127" t="s">
+      <c r="B26" s="123"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="127"/>
-      <c r="F26" s="127"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="123"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="122" t="s">
+      <c r="A27" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="131"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="136"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="121" t="s">
+      <c r="A28" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="121"/>
-      <c r="C28" s="121"/>
-      <c r="D28" s="122" t="s">
+      <c r="B28" s="130"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="131" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="122"/>
-      <c r="F28" s="122"/>
+      <c r="E28" s="131"/>
+      <c r="F28" s="131"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="123"/>
-      <c r="C29" s="123"/>
-      <c r="D29" s="124"/>
-      <c r="E29" s="124"/>
-      <c r="F29" s="124"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="133"/>
+      <c r="F29" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2740,6 +2739,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2754,8 +2763,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:C26"/>
+    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2767,11 +2776,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
     </row>
     <row r="3" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -3041,14 +3050,26 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="105"/>
+      <c r="A27" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B27" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="105" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="105"/>
+      <c r="A28" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B28" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="C28" s="105" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
@@ -3091,8 +3112,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,11 +3125,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3397,14 +3418,26 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B29" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="121" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="40">
+        <v>45348</v>
+      </c>
+      <c r="B30" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="C30" s="121" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="41"/>
@@ -3494,7 +3527,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3508,29 +3541,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="136"/>
+      <c r="C3" s="137"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="136"/>
+      <c r="C4" s="137"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="136"/>
+      <c r="C5" s="137"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3753,11 +3786,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -3765,18 +3798,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="139" t="s">
+      <c r="A4" s="140" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="139"/>
-      <c r="C4" s="139"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -4052,14 +4085,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4337,8 +4370,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4352,16 +4385,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="122" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4683,10 +4716,10 @@
         <v>4</v>
       </c>
       <c r="E18" s="56">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F18" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="58"/>
       <c r="H18" s="56"/>
@@ -4770,10 +4803,10 @@
         <v>3</v>
       </c>
       <c r="E23" s="65">
+        <v>3</v>
+      </c>
+      <c r="F23" s="65">
         <v>0</v>
-      </c>
-      <c r="F23" s="65">
-        <v>3</v>
       </c>
       <c r="G23" s="58"/>
       <c r="H23" s="65"/>
@@ -4991,11 +5024,11 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>13.25</v>
+        <v>19.25</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I35" s="71"/>
     </row>
@@ -5041,19 +5074,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="141" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
-      <c r="K1" s="140"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -5717,16 +5750,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -6502,71 +6535,71 @@
       <c r="A21" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="142" t="s">
+      <c r="B21" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="143"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="101" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="143" t="s">
+      <c r="B22" s="144" t="s">
         <v>188</v>
       </c>
-      <c r="C22" s="143"/>
-      <c r="D22" s="143"/>
+      <c r="C22" s="144"/>
+      <c r="D22" s="144"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>189</v>
       </c>
-      <c r="B23" s="143" t="s">
+      <c r="B23" s="144" t="s">
         <v>190</v>
       </c>
-      <c r="C23" s="143"/>
-      <c r="D23" s="143"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="101" t="s">
         <v>191</v>
       </c>
-      <c r="B24" s="143" t="s">
+      <c r="B24" s="144" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="143"/>
-      <c r="D24" s="143"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
-      <c r="B25" s="141"/>
-      <c r="C25" s="141"/>
-      <c r="D25" s="141"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="142"/>
+      <c r="D25" s="142"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="98"/>
-      <c r="B26" s="141"/>
-      <c r="C26" s="141"/>
-      <c r="D26" s="141"/>
+      <c r="B26" s="142"/>
+      <c r="C26" s="142"/>
+      <c r="D26" s="142"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="98"/>
-      <c r="B27" s="141"/>
-      <c r="C27" s="141"/>
-      <c r="D27" s="141"/>
+      <c r="B27" s="142"/>
+      <c r="C27" s="142"/>
+      <c r="D27" s="142"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
-      <c r="B28" s="141"/>
-      <c r="C28" s="141"/>
-      <c r="D28" s="141"/>
+      <c r="B28" s="142"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="142"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="98"/>
-      <c r="B29" s="141"/>
-      <c r="C29" s="141"/>
-      <c r="D29" s="141"/>
+      <c r="B29" s="142"/>
+      <c r="C29" s="142"/>
+      <c r="D29" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>